<commit_message>
Fixed gitignore for images
</commit_message>
<xml_diff>
--- a/SkySearchImages/SkySearch Images.xlsx
+++ b/SkySearchImages/SkySearch Images.xlsx
@@ -358,7 +358,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -372,6 +372,13 @@
     </fill>
   </fills>
   <borders count="3">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -394,29 +401,22 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">

</xml_diff>

<commit_message>
Minor modifications to some image processing in the result analysis notebook
</commit_message>
<xml_diff>
--- a/SkySearchImages/SkySearch Images.xlsx
+++ b/SkySearchImages/SkySearch Images.xlsx
@@ -342,19 +342,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -410,13 +404,13 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">

</xml_diff>